<commit_message>
All Monk archetypes added to the program, limited spell casting method also added for future use.
</commit_message>
<xml_diff>
--- a/lib/classes/AttackAndSpellCastingLevelIncr.xlsx
+++ b/lib/classes/AttackAndSpellCastingLevelIncr.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="54">
   <si>
     <t>Channel Divinity</t>
   </si>
@@ -19,30 +19,60 @@
     <t>Destroy Undead</t>
   </si>
   <si>
+    <t>Fists of Bone and Steel</t>
+  </si>
+  <si>
+    <t>Ki</t>
+  </si>
+  <si>
+    <t>Martial Arts</t>
+  </si>
+  <si>
     <t>Psionic Power</t>
   </si>
   <si>
+    <t>Radiant Sun Bolt</t>
+  </si>
+  <si>
     <t>Sneak Attack</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
+    <t>1d4</t>
+  </si>
+  <si>
     <t>1d6</t>
   </si>
   <si>
     <t>x1</t>
   </si>
   <si>
+    <t>2 points</t>
+  </si>
+  <si>
+    <t>3 points</t>
+  </si>
+  <si>
     <t>d6</t>
   </si>
   <si>
     <t>2d6</t>
   </si>
   <si>
+    <t>4 points</t>
+  </si>
+  <si>
     <t>CR 1/2</t>
   </si>
   <si>
+    <t>1d8</t>
+  </si>
+  <si>
+    <t>5 points</t>
+  </si>
+  <si>
     <t>d8</t>
   </si>
   <si>
@@ -52,36 +82,78 @@
     <t>x2</t>
   </si>
   <si>
+    <t>6 points</t>
+  </si>
+  <si>
+    <t>7 points</t>
+  </si>
+  <si>
     <t>4d6</t>
   </si>
   <si>
     <t>CR 1</t>
   </si>
   <si>
+    <t>8 points</t>
+  </si>
+  <si>
+    <t>9 points</t>
+  </si>
+  <si>
     <t>5d6</t>
   </si>
   <si>
+    <t>10 points</t>
+  </si>
+  <si>
     <t>CR 2</t>
   </si>
   <si>
+    <t>1d10</t>
+  </si>
+  <si>
+    <t>11 points</t>
+  </si>
+  <si>
     <t>d10</t>
   </si>
   <si>
     <t>6d6</t>
   </si>
   <si>
+    <t>12 points</t>
+  </si>
+  <si>
+    <t>13 points</t>
+  </si>
+  <si>
     <t>7d6</t>
   </si>
   <si>
     <t>CR 3</t>
   </si>
   <si>
+    <t>14 points</t>
+  </si>
+  <si>
+    <t>15 points</t>
+  </si>
+  <si>
     <t>8d6</t>
   </si>
   <si>
+    <t>16 points</t>
+  </si>
+  <si>
     <t>CR 4</t>
   </si>
   <si>
+    <t>1d12</t>
+  </si>
+  <si>
+    <t>17 points</t>
+  </si>
+  <si>
     <t>d12</t>
   </si>
   <si>
@@ -91,7 +163,16 @@
     <t>x3</t>
   </si>
   <si>
+    <t>18 points</t>
+  </si>
+  <si>
+    <t>19 points</t>
+  </si>
+  <si>
     <t>10d6</t>
+  </si>
+  <si>
+    <t>20 points</t>
   </si>
 </sst>
 </file>
@@ -368,285 +449,537 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>19</v>
+        <v>39</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>21</v>
+        <v>39</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>17</v>
+        <v>39</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>24</v>
+        <v>46</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>24</v>
+        <v>50</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>26</v>
+        <v>51</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>26</v>
+        <v>53</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>